<commit_message>
Update to add new method in sheets and add integration tests
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/config_1.xlsx
+++ b/tests/integration_test_files/config_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4FC7A2E-692C-9D4C-AD6F-A5363925FE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEB86D0-E514-0541-A320-5A556EA74297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="66420" yWindow="2040" windowWidth="33260" windowHeight="19480" firstSheet="5" activeTab="14" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="24540" yWindow="500" windowWidth="33260" windowHeight="19480" firstSheet="2" activeTab="11" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="291">
   <si>
     <t>Epoch</t>
   </si>
@@ -292,9 +292,6 @@
     <t>BOTH</t>
   </si>
   <si>
-    <t>Pop 2</t>
-  </si>
-  <si>
     <t>60 years</t>
   </si>
   <si>
@@ -376,9 +373,6 @@
     <t>Time to recovery, defined as discharged or “ready for discharge” (as evidenced by normal body temperature and respiratory rate, and stable oxygen saturation on ambient air or &lt;= 2L supplemental oxygen); OR, in a non-ICU hospital ward (or “ready for hospital ward”) not requiring supplemental oxygen</t>
   </si>
   <si>
-    <t>Duration of supplemental oxygen</t>
-  </si>
-  <si>
     <t>Secondary Endpoint</t>
   </si>
   <si>
@@ -799,9 +793,6 @@
     <t>Treatment Element 1</t>
   </si>
   <si>
-    <t>Treatment Element 2</t>
-  </si>
-  <si>
     <t>Completed treatment 1</t>
   </si>
   <si>
@@ -832,9 +823,6 @@
     <t>Test9</t>
   </si>
   <si>
-    <t>Test Eight</t>
-  </si>
-  <si>
     <t>Test Nine</t>
   </si>
   <si>
@@ -865,9 +853,6 @@
     <t>TREATMENT</t>
   </si>
   <si>
-    <t>Follow-up Epoch</t>
-  </si>
-  <si>
     <t>FOLLOW-UP</t>
   </si>
   <si>
@@ -913,13 +898,31 @@
     <t>activityIsConditionalReason</t>
   </si>
   <si>
-    <t>Basic Demog</t>
-  </si>
-  <si>
     <t>Something weird</t>
   </si>
   <si>
     <t>Only do this if they have two heads</t>
+  </si>
+  <si>
+    <t>Sdr PREV NEXT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDR </t>
+  </si>
+  <si>
+    <t>sdr root</t>
+  </si>
+  <si>
+    <t>sdr DESCRIPTIOn</t>
+  </si>
+  <si>
+    <t>No description set</t>
+  </si>
+  <si>
+    <t>OBJ3</t>
+  </si>
+  <si>
+    <t>END13</t>
   </si>
 </sst>
 </file>
@@ -1059,10 +1062,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1456,10 +1459,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>142</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>144</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
@@ -1470,10 +1473,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>143</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>145</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
@@ -1484,10 +1487,10 @@
     </row>
     <row r="7" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
@@ -1508,42 +1511,42 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="C9" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="D9" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="E9" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="F9" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="G9" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="H9" s="21" t="s">
         <v>151</v>
-      </c>
-      <c r="G9" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="H9" s="21" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="D10" s="11" t="s">
         <v>155</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>157</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -1553,33 +1556,33 @@
         <v>40179</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>156</v>
-      </c>
       <c r="D11" s="11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G11" s="15">
         <v>40544</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1671,8 +1674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B908C5D6-C6A1-4043-A49A-69C599CFBAE9}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1686,214 +1689,222 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>90</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" s="10" t="s">
+      <c r="E2" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="E2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>94</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C3" s="10" t="s">
+      <c r="E3" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>98</v>
-      </c>
       <c r="G3" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>108</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>289</v>
+      </c>
       <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
+      <c r="C14" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" s="10"/>
@@ -2081,7 +2092,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFC82B4-C495-A142-993D-B6A47D77A4C3}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -2097,90 +2108,90 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>72</v>
       </c>
       <c r="D1" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>134</v>
-      </c>
       <c r="G1" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" t="s">
         <v>135</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>139</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H2" t="s">
         <v>136</v>
-      </c>
-      <c r="D2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E2" t="s">
-        <v>141</v>
-      </c>
-      <c r="F2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" t="s">
         <v>172</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E5" t="s">
         <v>173</v>
       </c>
-      <c r="C5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
+        <v>112</v>
+      </c>
+      <c r="G5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H5" t="s">
         <v>174</v>
-      </c>
-      <c r="E5" t="s">
-        <v>175</v>
-      </c>
-      <c r="F5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G5" t="s">
-        <v>120</v>
-      </c>
-      <c r="H5" t="s">
-        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2192,8 +2203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D608A778-255D-4443-A7EA-03049F1FC98F}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2209,65 +2220,62 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B1" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="F1" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>256</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>257</v>
-      </c>
-      <c r="E1" s="18" t="s">
+      <c r="G1" s="18" t="s">
         <v>189</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>190</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C2" t="s">
+        <v>255</v>
+      </c>
+      <c r="E2" t="s">
         <v>192</v>
-      </c>
-      <c r="B2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C2" t="s">
-        <v>258</v>
-      </c>
-      <c r="D2" t="s">
-        <v>260</v>
-      </c>
-      <c r="E2" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C3" t="s">
+        <v>256</v>
+      </c>
+      <c r="D3" t="s">
+        <v>257</v>
+      </c>
+      <c r="E3" t="s">
+        <v>194</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="B3" t="s">
-        <v>193</v>
-      </c>
-      <c r="C3" t="s">
-        <v>259</v>
-      </c>
-      <c r="D3" t="s">
-        <v>261</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>196</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="G3" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -2300,137 +2308,137 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B1" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="D1" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="E1" s="24" t="s">
         <v>201</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="F1" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="G1" s="24" t="s">
         <v>203</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="H1" s="24" t="s">
         <v>204</v>
-      </c>
-      <c r="G1" s="24" t="s">
-        <v>205</v>
-      </c>
-      <c r="H1" s="24" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>215</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>213</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>215</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>212</v>
-      </c>
       <c r="E5" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>213</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>214</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -2444,7 +2452,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2457,104 +2465,101 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>240</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>241</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>248</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>232</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>236</v>
-      </c>
       <c r="C5" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -2565,31 +2570,56 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1886B59F-3C17-014D-9C61-BEC33F421A82}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" t="s">
         <v>167</v>
-      </c>
-      <c r="B1" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B2" t="s">
-        <v>168</v>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B3" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B4" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -2645,7 +2675,7 @@
         <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E2" t="s">
         <v>39</v>
@@ -2665,7 +2695,7 @@
         <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E3" t="s">
         <v>55</v>
@@ -2696,10 +2726,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
@@ -2707,10 +2737,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
@@ -2720,41 +2750,41 @@
       <c r="A3" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="26" t="s">
-        <v>179</v>
-      </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
+      <c r="B3" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="27" t="s">
-        <v>199</v>
-      </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
+      <c r="B4" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="27" t="s">
-        <v>163</v>
-      </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
+      <c r="B5" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>48</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
@@ -2765,7 +2795,7 @@
         <v>50</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -2776,7 +2806,7 @@
         <v>49</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C8" s="25"/>
       <c r="D8" s="25"/>
@@ -2784,10 +2814,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C9" s="25"/>
       <c r="D9" s="25"/>
@@ -2795,7 +2825,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B10" s="25"/>
       <c r="C10" s="25"/>
@@ -2804,7 +2834,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>43</v>
@@ -2824,16 +2854,16 @@
         <v>41</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C13" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>232</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -2841,16 +2871,16 @@
         <v>42</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C14" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>232</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -2867,16 +2897,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2887,7 +2917,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2901,19 +2931,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2921,33 +2951,30 @@
         <v>41</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2963,7 +2990,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2975,13 +3002,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2989,10 +3016,10 @@
         <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -3000,10 +3027,10 @@
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -3011,21 +3038,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>271</v>
-      </c>
+      <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -3055,10 +3080,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>0</v>
@@ -3079,10 +3104,10 @@
     </row>
     <row r="2" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>3</v>
@@ -3105,10 +3130,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>21</v>
@@ -3199,29 +3224,29 @@
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="17" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="17" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>15</v>
@@ -3242,7 +3267,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -3311,7 +3336,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3325,38 +3350,35 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>287</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D3" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3373,7 +3395,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3384,7 +3406,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>61</v>
@@ -3398,7 +3420,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
         <v>62</v>
@@ -3412,7 +3434,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B3" t="s">
         <v>63</v>
@@ -3426,7 +3448,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s">
         <v>62</v>
@@ -3440,13 +3462,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B5" t="s">
         <v>63</v>
-      </c>
-      <c r="C5" t="s">
-        <v>68</v>
       </c>
       <c r="D5" t="s">
         <v>71</v>
@@ -3462,7 +3481,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3485,7 +3504,7 @@
         <v>75</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>78</v>
@@ -3511,9 +3530,6 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>80</v>
-      </c>
       <c r="B3">
         <v>20</v>
       </c>
@@ -3521,15 +3537,15 @@
         <v>76</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" t="s">
         <v>81</v>
-      </c>
-      <c r="E3" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4">
         <v>20</v>
@@ -3538,10 +3554,10 @@
         <v>76</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" t="s">
         <v>84</v>
-      </c>
-      <c r="E4" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update tests and field handling
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/config_1.xlsx
+++ b/tests/integration_test_files/config_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3855056-4924-BD4B-AC52-D872F08738CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A000A90-1282-8548-8A78-EFB55DB3F1F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24540" yWindow="500" windowWidth="44440" windowHeight="23580" firstSheet="1" activeTab="9" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="24540" yWindow="500" windowWidth="44440" windowHeight="23580" firstSheet="3" activeTab="15" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="335">
   <si>
     <t>Epoch</t>
   </si>
@@ -1050,6 +1050,12 @@
   </si>
   <si>
     <t>31 years</t>
+  </si>
+  <si>
+    <t>empty none</t>
+  </si>
+  <si>
+    <t>empty</t>
   </si>
 </sst>
 </file>
@@ -1188,10 +1194,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1663,7 +1669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C037A932-CB5B-8D43-956E-5F5C367E07FC}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection sqref="A1:I1048576"/>
     </sheetView>
   </sheetViews>
@@ -2807,10 +2813,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1886B59F-3C17-014D-9C61-BEC33F421A82}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2857,6 +2863,14 @@
       </c>
       <c r="B5" s="6" t="s">
         <v>266</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="B6" t="s">
+        <v>334</v>
       </c>
     </row>
   </sheetData>
@@ -2987,34 +3001,34 @@
       <c r="A3" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="25" t="s">
         <v>175</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
@@ -3134,16 +3148,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>